<commit_message>
Add to cart case added
</commit_message>
<xml_diff>
--- a/HackerRankTest4/configs/LoginData.xlsx
+++ b/HackerRankTest4/configs/LoginData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raheel\git\repository3\HackerRankTest4\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A16148-DDE2-4759-BB0A-D7845EEF049E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA1F859-6C6D-4A45-9D9E-0666BDB278EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,38 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>dasdas</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>JaysonOlson1@gmail.com</t>
-  </si>
-  <si>
-    <t>JaysonOlson2@gmail.com</t>
-  </si>
-  <si>
-    <t>JaysonOlson3@gmail.com</t>
-  </si>
-  <si>
-    <t>JaysonOlson4@gmail.com</t>
-  </si>
-  <si>
-    <t>JaysonOlson5@gmail.com</t>
+    <t>mukraheel@gmail.com</t>
+  </si>
+  <si>
+    <t>R@heel123</t>
+  </si>
+  <si>
+    <t>Raheel1234</t>
+  </si>
+  <si>
+    <t>Testmail@gmail.com</t>
+  </si>
+  <si>
+    <t>test123456</t>
+  </si>
+  <si>
+    <t>accraheel123@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,15 +377,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -394,23 +394,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -418,32 +418,15 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{29848C19-A008-4FE8-A0F3-74BC4DB8AA56}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{A7C3826B-F469-48ED-84F9-49BF101846AC}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{E76BC697-4054-4DA9-9916-4F282241BCC5}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{9BC1C87C-5077-4C7A-BCF2-CC476EF05836}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{8B33CABA-0400-4AF6-A12B-1295117011DC}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{9BC1C87C-5077-4C7A-BCF2-CC476EF05836}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{DAE63CD2-0082-45E9-864E-5913E5A3BFFB}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{18E889DD-4505-4CC6-B1E4-BC04F614363A}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{A98B602E-A730-46AD-B9EA-892128728E47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>